<commit_message>
refactored testing with Steps Epoch import
</commit_message>
<xml_diff>
--- a/fixtures/Ciclid Brain and Social Data with Legend.xlsx
+++ b/fixtures/Ciclid Brain and Social Data with Legend.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="24560" windowHeight="15620" tabRatio="890" activeTab="2"/>
+    <workbookView xWindow="16880" yWindow="500" windowWidth="31280" windowHeight="16060" tabRatio="890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Huber et al., 1997" sheetId="4" r:id="rId1"/>
@@ -2153,12 +2153,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="36"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="17"/>
       <name val="Calibri"/>
@@ -2184,12 +2178,6 @@
       <color indexed="56"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2284,8 +2272,22 @@
       <color indexed="10"/>
       <name val="Arial Black"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2411,6 +2413,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3366FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2560,7 +2568,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="46">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2590,78 +2598,77 @@
     <xf numFmtId="0" fontId="7" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="39"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="37"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="37" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="39" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="37" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="37" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="39" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="39" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="40" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="40" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="40" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="40" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="40" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="40" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="40" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="40" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="40"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="38" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="38" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="38" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="38" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="38" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="38" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="38" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="38" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="38"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="40" applyFont="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="40" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="38" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="38" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="39" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="37" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2670,10 +2677,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="46">
+  <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="1"/>
     <cellStyle name="20% - Accent2" xfId="2"/>
     <cellStyle name="20% - Accent3" xfId="3"/>
@@ -2702,24 +2708,26 @@
     <cellStyle name="Calculation" xfId="26"/>
     <cellStyle name="Check Cell" xfId="27"/>
     <cellStyle name="Explanatory Text" xfId="28"/>
-    <cellStyle name="Followed Hyperlink_Data Consilidation.xls" xfId="29"/>
-    <cellStyle name="Good" xfId="30"/>
-    <cellStyle name="Heading 1" xfId="31"/>
-    <cellStyle name="Heading 2" xfId="32"/>
-    <cellStyle name="Heading 3" xfId="33"/>
-    <cellStyle name="Heading 4" xfId="34"/>
-    <cellStyle name="Hyperlink_Data Consilidation.xls" xfId="35"/>
-    <cellStyle name="Input" xfId="36"/>
-    <cellStyle name="Linked Cell" xfId="37"/>
-    <cellStyle name="Neutral" xfId="38"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="29"/>
+    <cellStyle name="Heading 1" xfId="30"/>
+    <cellStyle name="Heading 2" xfId="31"/>
+    <cellStyle name="Heading 3" xfId="32"/>
+    <cellStyle name="Heading 4" xfId="33"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Input" xfId="34"/>
+    <cellStyle name="Linked Cell" xfId="35"/>
+    <cellStyle name="Neutral" xfId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Data Consilidation.xls" xfId="39"/>
-    <cellStyle name="Normal_TOTAL DATA.xls" xfId="40"/>
-    <cellStyle name="Note" xfId="41"/>
-    <cellStyle name="Output" xfId="42"/>
-    <cellStyle name="Title" xfId="43"/>
-    <cellStyle name="Total" xfId="44"/>
-    <cellStyle name="Warning Text" xfId="45"/>
+    <cellStyle name="Normal_Data Consilidation.xls" xfId="37"/>
+    <cellStyle name="Normal_TOTAL DATA.xls" xfId="38"/>
+    <cellStyle name="Note" xfId="39"/>
+    <cellStyle name="Output" xfId="40"/>
+    <cellStyle name="Title" xfId="41"/>
+    <cellStyle name="Total" xfId="42"/>
+    <cellStyle name="Warning Text" xfId="43"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -2993,11 +3001,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="560797112"/>
-        <c:axId val="560803304"/>
+        <c:axId val="620488984"/>
+        <c:axId val="620080936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="560797112"/>
+        <c:axId val="620488984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3071,12 +3079,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="560803304"/>
+        <c:crossAx val="620080936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="560803304"/>
+        <c:axId val="620080936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3160,7 +3168,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="560797112"/>
+        <c:crossAx val="620488984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -28950,7 +28958,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -28958,7 +28966,11 @@
     <col min="1" max="1" width="8.83203125" style="15"/>
     <col min="2" max="2" width="19.6640625" style="15" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="15" customWidth="1"/>
-    <col min="4" max="28" width="8.83203125" style="15"/>
+    <col min="4" max="18" width="8.83203125" style="15"/>
+    <col min="19" max="20" width="12.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="28" width="8.83203125" style="15"/>
     <col min="29" max="29" width="8.5" style="15" customWidth="1"/>
     <col min="30" max="33" width="8.83203125" style="15"/>
     <col min="34" max="34" width="11.6640625" style="15" customWidth="1"/>
@@ -28979,103 +28991,103 @@
       <c r="A1" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="41" t="s">
         <v>661</v>
       </c>
-      <c r="I1" s="44" t="s">
+      <c r="I1" s="40" t="s">
         <v>662</v>
       </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="40" t="s">
         <v>663</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="40" t="s">
         <v>117</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="M1" s="40" t="s">
         <v>664</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="N1" s="40" t="s">
         <v>246</v>
       </c>
-      <c r="O1" s="44" t="s">
+      <c r="O1" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="40" t="s">
         <v>665</v>
       </c>
-      <c r="Q1" s="44" t="s">
+      <c r="Q1" s="40" t="s">
         <v>434</v>
       </c>
-      <c r="R1" s="44" t="s">
+      <c r="R1" s="40" t="s">
         <v>435</v>
       </c>
-      <c r="S1" s="44" t="s">
+      <c r="S1" s="40" t="s">
         <v>436</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="T1" s="46" t="s">
         <v>437</v>
       </c>
-      <c r="U1" s="44" t="s">
+      <c r="U1" s="46" t="s">
         <v>417</v>
       </c>
-      <c r="V1" s="44" t="s">
+      <c r="V1" s="46" t="s">
         <v>438</v>
       </c>
-      <c r="W1" s="44" t="s">
+      <c r="W1" s="40" t="s">
         <v>439</v>
       </c>
-      <c r="X1" s="44" t="s">
+      <c r="X1" s="46" t="s">
         <v>440</v>
       </c>
-      <c r="Y1" s="44" t="s">
+      <c r="Y1" s="46" t="s">
         <v>162</v>
       </c>
-      <c r="Z1" s="44" t="s">
+      <c r="Z1" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="AA1" s="44" t="s">
+      <c r="AA1" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="AB1" s="44" t="s">
+      <c r="AB1" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="44" t="s">
+      <c r="AC1" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="44" t="s">
+      <c r="AD1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="44" t="s">
+      <c r="AE1" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="44" t="s">
+      <c r="AF1" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="44" t="s">
+      <c r="AG1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="44" t="s">
+      <c r="AH1" s="40" t="s">
         <v>28</v>
       </c>
       <c r="AI1" s="14" t="s">
@@ -50064,7 +50076,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -50523,17 +50535,17 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="42"/>
     </row>
     <row r="44" spans="1:9" ht="15" thickBot="1"/>
     <row r="45" spans="1:9">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="43"/>
       <c r="C45" t="s">
         <v>238</v>
       </c>
@@ -56555,7 +56567,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="19"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -58875,7 +58887,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21"/>
+  <phoneticPr fontId="19"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -58914,30 +58926,30 @@
       <c r="B2" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="42"/>
-      <c r="L2" s="41" t="s">
+      <c r="K2" s="45"/>
+      <c r="L2" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="M2" s="42"/>
-      <c r="N2" s="41" t="s">
+      <c r="M2" s="45"/>
+      <c r="N2" s="44" t="s">
         <v>491</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="41" t="s">
+      <c r="O2" s="45"/>
+      <c r="P2" s="44" t="s">
         <v>215</v>
       </c>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="41" t="s">
+      <c r="Q2" s="45"/>
+      <c r="R2" s="44" t="s">
         <v>206</v>
       </c>
-      <c r="S2" s="42"/>
+      <c r="S2" s="45"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
@@ -60683,7 +60695,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Normalized and test fixtures
</commit_message>
<xml_diff>
--- a/fixtures/Ciclid Brain and Social Data with Legend.xlsx
+++ b/fixtures/Ciclid Brain and Social Data with Legend.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16880" yWindow="500" windowWidth="31280" windowHeight="16060" tabRatio="890" activeTab="2"/>
+    <workbookView xWindow="16880" yWindow="500" windowWidth="31660" windowHeight="25140" tabRatio="890" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Huber et al., 1997" sheetId="4" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Legend" sheetId="5" r:id="rId8"/>
     <sheet name="Pearson's Correlations" sheetId="34" r:id="rId9"/>
     <sheet name="sheet 3" sheetId="3" r:id="rId10"/>
+    <sheet name="TestData" sheetId="35" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Pearson''s Correlations'!$A$1:$I$9</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7219" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7384" uniqueCount="684">
   <si>
     <t>Fatlipped Insectivore</t>
   </si>
@@ -2568,7 +2569,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2613,6 +2614,8 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2667,6 +2670,7 @@
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2677,9 +2681,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="50">
     <cellStyle name="20% - Accent1" xfId="1"/>
     <cellStyle name="20% - Accent2" xfId="2"/>
     <cellStyle name="20% - Accent3" xfId="3"/>
@@ -2710,6 +2713,7 @@
     <cellStyle name="Explanatory Text" xfId="28"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="29"/>
     <cellStyle name="Heading 1" xfId="30"/>
     <cellStyle name="Heading 2" xfId="31"/>
@@ -2717,6 +2721,7 @@
     <cellStyle name="Heading 4" xfId="33"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="34"/>
     <cellStyle name="Linked Cell" xfId="35"/>
     <cellStyle name="Neutral" xfId="36"/>
@@ -3001,11 +3006,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="620488984"/>
-        <c:axId val="620080936"/>
+        <c:axId val="112209480"/>
+        <c:axId val="113134744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="620488984"/>
+        <c:axId val="112209480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3079,12 +3084,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="620080936"/>
+        <c:crossAx val="113134744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="620080936"/>
+        <c:axId val="113134744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,7 +3173,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="620488984"/>
+        <c:crossAx val="112209480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -21019,6 +21024,1196 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:34">
+      <c r="A1" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>661</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>662</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>663</v>
+      </c>
+      <c r="K1" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="40" t="s">
+        <v>664</v>
+      </c>
+      <c r="N1" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="O1" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="40" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q1" s="40" t="s">
+        <v>434</v>
+      </c>
+      <c r="R1" s="40" t="s">
+        <v>435</v>
+      </c>
+      <c r="S1" s="40" t="s">
+        <v>436</v>
+      </c>
+      <c r="T1" s="42" t="s">
+        <v>437</v>
+      </c>
+      <c r="U1" s="42" t="s">
+        <v>417</v>
+      </c>
+      <c r="V1" s="42" t="s">
+        <v>438</v>
+      </c>
+      <c r="W1" s="40" t="s">
+        <v>439</v>
+      </c>
+      <c r="X1" s="42" t="s">
+        <v>440</v>
+      </c>
+      <c r="Y1" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z1" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="AA1" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH1" s="40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34">
+      <c r="A2" s="13"/>
+      <c r="B2" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+    </row>
+    <row r="3" spans="1:34">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11" t="s">
+        <v>580</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+    </row>
+    <row r="4" spans="1:34">
+      <c r="A4" s="15">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="15">
+        <v>29</v>
+      </c>
+      <c r="F4" s="15">
+        <v>0</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15">
+        <v>12.322295614789493</v>
+      </c>
+      <c r="J4" s="15">
+        <v>69.05</v>
+      </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15">
+        <v>8.1667000000000005</v>
+      </c>
+      <c r="N4" s="15">
+        <v>0.10814585673160364</v>
+      </c>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15">
+        <v>0.32573999999999997</v>
+      </c>
+      <c r="Q4" s="15">
+        <v>4.0829897799209033E-4</v>
+      </c>
+      <c r="R4" s="15">
+        <v>2.4100060856861037E-3</v>
+      </c>
+      <c r="S4" s="15">
+        <v>6.1127083900873319E-3</v>
+      </c>
+      <c r="T4" s="15" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="W4" s="15">
+        <v>4.2235215434520785E-3</v>
+      </c>
+      <c r="X4" s="15">
+        <v>4.6577284548102171E-4</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z4" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA4" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="AB4" s="15"/>
+      <c r="AC4" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="AD4" s="15"/>
+      <c r="AE4" s="15" t="s">
+        <v>420</v>
+      </c>
+      <c r="AF4" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="AG4" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="AH4" s="15" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
+      <c r="A5" s="15">
+        <v>2</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="15">
+        <v>54</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15">
+        <v>16.671034161982281</v>
+      </c>
+      <c r="J5" s="15">
+        <v>68.47</v>
+      </c>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15">
+        <v>7.6775700000000002</v>
+      </c>
+      <c r="N5" s="15">
+        <v>9.3247054797434073E-2</v>
+      </c>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15">
+        <v>0.67569000000000001</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>3.701734734000865E-4</v>
+      </c>
+      <c r="R5" s="15">
+        <v>4.1452234597834994E-3</v>
+      </c>
+      <c r="S5" s="15">
+        <v>8.3555377234440127E-3</v>
+      </c>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15">
+        <v>4.4125211072159583E-3</v>
+      </c>
+      <c r="X5" s="15">
+        <v>4.370398224672612E-4</v>
+      </c>
+      <c r="Y5" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="Z5" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="AA5" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="AF5" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="AG5" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="AH5" s="15" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34">
+      <c r="A6" s="15">
+        <v>3</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="15">
+        <v>65</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15">
+        <v>6.3873985956755845</v>
+      </c>
+      <c r="J6" s="15">
+        <v>85.34</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15">
+        <v>8.0916300000000003</v>
+      </c>
+      <c r="N6" s="15">
+        <v>0.10577535173065575</v>
+      </c>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15">
+        <v>0.35011999999999999</v>
+      </c>
+      <c r="Q6" s="15" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R6" s="15">
+        <v>1.8655112240433475E-3</v>
+      </c>
+      <c r="S6" s="15">
+        <v>3.3848026866201922E-3</v>
+      </c>
+      <c r="T6" s="15">
+        <v>1.9846337960708867E-3</v>
+      </c>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15">
+        <v>2.160803865566979E-3</v>
+      </c>
+      <c r="X6" s="15">
+        <v>6.6078616768912933E-5</v>
+      </c>
+      <c r="Y6" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z6" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="AA6" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="AF6" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="AG6" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="AH6" s="15" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34">
+      <c r="A7" s="15">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="15">
+        <v>25</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15">
+        <v>5.8862686342018256</v>
+      </c>
+      <c r="J7" s="15">
+        <v>57.61</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15">
+        <v>5.3029999999999999</v>
+      </c>
+      <c r="N7" s="15">
+        <v>3.8366302360533809E-2</v>
+      </c>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15">
+        <v>3.9197755441064729E-3</v>
+      </c>
+      <c r="S7" s="15">
+        <v>8.8516786513094057E-3</v>
+      </c>
+      <c r="T7" s="15">
+        <v>5.9992958304727027E-3</v>
+      </c>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="W7" s="15">
+        <v>3.9938405306974133E-3</v>
+      </c>
+      <c r="X7" s="15" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y7" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z7" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA7" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="AF7" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="AG7" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH7" s="15" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34">
+      <c r="A8" s="15">
+        <v>5</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>649</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="15">
+        <v>58</v>
+      </c>
+      <c r="F8" s="15">
+        <v>1</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="H8" s="15">
+        <v>25019</v>
+      </c>
+      <c r="I8" s="15">
+        <v>8.4041542726555303</v>
+      </c>
+      <c r="J8" s="15">
+        <v>66.81</v>
+      </c>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15">
+        <v>7.953241345287243E-3</v>
+      </c>
+      <c r="S8" s="15">
+        <v>1.4796446604885728E-2</v>
+      </c>
+      <c r="T8" s="15">
+        <v>5.999713668485453E-3</v>
+      </c>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15">
+        <v>9.5746053037342183E-3</v>
+      </c>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z8" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA8" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="AF8" s="15" t="s">
+        <v>651</v>
+      </c>
+      <c r="AG8" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH8" s="15" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34">
+      <c r="A9" s="15">
+        <v>6</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>652</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="15">
+        <v>66</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="H9" s="15">
+        <v>25253</v>
+      </c>
+      <c r="I9" s="15">
+        <v>22.423802683523043</v>
+      </c>
+      <c r="J9" s="15">
+        <v>70.7</v>
+      </c>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15">
+        <v>8.3349899999999995</v>
+      </c>
+      <c r="N9" s="15">
+        <v>0.11357172952737067</v>
+      </c>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15">
+        <v>0.40325</v>
+      </c>
+      <c r="Q9" s="15">
+        <v>3.5973080989898886E-4</v>
+      </c>
+      <c r="R9" s="15">
+        <v>6.6096185898674026E-3</v>
+      </c>
+      <c r="S9" s="15">
+        <v>9.3355908171142161E-3</v>
+      </c>
+      <c r="T9" s="15">
+        <v>4.4564201588857075E-3</v>
+      </c>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15">
+        <v>2.1810943584757377E-4</v>
+      </c>
+      <c r="W9" s="15">
+        <v>6.8179223228907043E-3</v>
+      </c>
+      <c r="X9" s="15">
+        <v>7.2167854016910184E-4</v>
+      </c>
+      <c r="Y9" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z9" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA9" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="AB9" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="AC9" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="AD9" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="AE9" s="15" t="s">
+        <v>648</v>
+      </c>
+      <c r="AF9" s="15" t="s">
+        <v>651</v>
+      </c>
+      <c r="AG9" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="AH9" s="15" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34">
+      <c r="A10" s="15">
+        <v>7</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="15">
+        <v>59</v>
+      </c>
+      <c r="F10" s="15">
+        <v>0</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15">
+        <v>10.559694197054334</v>
+      </c>
+      <c r="J10" s="15">
+        <v>85.35</v>
+      </c>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15">
+        <v>9.1338699999999999</v>
+      </c>
+      <c r="N10" s="15">
+        <v>0.14147171642170334</v>
+      </c>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15">
+        <v>3.782045953762948E-5</v>
+      </c>
+      <c r="R10" s="15">
+        <v>1.0699939648646321E-2</v>
+      </c>
+      <c r="S10" s="15">
+        <v>1.7295750612067E-2</v>
+      </c>
+      <c r="T10" s="15">
+        <v>8.5128878107509076E-3</v>
+      </c>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15">
+        <v>3.2135827935560315E-4</v>
+      </c>
+      <c r="W10" s="15">
+        <v>9.4623824140948835E-3</v>
+      </c>
+      <c r="X10" s="15">
+        <v>3.1926967554462069E-4</v>
+      </c>
+      <c r="Y10" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z10" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA10" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="AB10" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="15" t="s">
+        <v>420</v>
+      </c>
+      <c r="AF10" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="AG10" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="AH10" s="15" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34">
+      <c r="A11" s="15">
+        <v>8</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="15">
+        <v>77</v>
+      </c>
+      <c r="F11" s="15">
+        <v>0</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15">
+        <v>84.909878354812875</v>
+      </c>
+      <c r="J11" s="15">
+        <v>71.33</v>
+      </c>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15">
+        <v>8.3052299999999999</v>
+      </c>
+      <c r="N11" s="15">
+        <v>0.11260094458017346</v>
+      </c>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15">
+        <v>0.12504000000000001</v>
+      </c>
+      <c r="Q11" s="15" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R11" s="15">
+        <v>1.3768562612273551E-2</v>
+      </c>
+      <c r="S11" s="15">
+        <v>2.1858604119013254E-2</v>
+      </c>
+      <c r="T11" s="15">
+        <v>8.1597131567683317E-3</v>
+      </c>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="W11" s="15" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="X11" s="15">
+        <v>8.7074327881756538E-4</v>
+      </c>
+      <c r="Y11" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="Z11" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="AA11" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="AF11" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG11" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="AH11" s="15" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34">
+      <c r="A12" s="15">
+        <v>9</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="15">
+        <v>74</v>
+      </c>
+      <c r="F12" s="15">
+        <v>1</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15">
+        <v>28.365862998319251</v>
+      </c>
+      <c r="J12" s="15">
+        <v>131.63</v>
+      </c>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15">
+        <v>5.1116825638517728E-3</v>
+      </c>
+      <c r="S12" s="15">
+        <v>9.4909846429057174E-3</v>
+      </c>
+      <c r="T12" s="15">
+        <v>5.6665366388506753E-3</v>
+      </c>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15">
+        <v>1.2227565046980342E-3</v>
+      </c>
+      <c r="Y12" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z12" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="AA12" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="AF12" s="15" t="s">
+        <v>651</v>
+      </c>
+      <c r="AG12" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="AH12" s="15" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34">
+      <c r="A13" s="15"/>
+      <c r="B13" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>582</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="15"/>
+      <c r="AF13" s="15"/>
+      <c r="AG13" s="15"/>
+      <c r="AH13" s="15"/>
+    </row>
+    <row r="14" spans="1:34">
+      <c r="A14" s="15">
+        <v>10</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="E14" s="15">
+        <v>56</v>
+      </c>
+      <c r="F14" s="15">
+        <v>0</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="H14" s="15">
+        <v>265468</v>
+      </c>
+      <c r="I14" s="15">
+        <v>9.3002238819061951</v>
+      </c>
+      <c r="J14" s="15">
+        <v>102.01</v>
+      </c>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15">
+        <v>9.36843</v>
+      </c>
+      <c r="N14" s="15">
+        <v>0.15034825737271287</v>
+      </c>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15">
+        <v>0.32241999999999998</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>3.2859874024052023E-4</v>
+      </c>
+      <c r="R14" s="15">
+        <v>7.1510853919616044E-3</v>
+      </c>
+      <c r="S14" s="15">
+        <v>8.8527468615720029E-3</v>
+      </c>
+      <c r="T14" s="15">
+        <v>4.3129978472854396E-3</v>
+      </c>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="W14" s="15">
+        <v>6.9801193344609241E-3</v>
+      </c>
+      <c r="X14" s="15">
+        <v>2.4857020048970485E-4</v>
+      </c>
+      <c r="Y14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z14" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="AA14" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="AB14" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="AF14" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="AG14" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="AH14" s="15" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34">
+      <c r="A15" s="15">
+        <v>11</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="E15" s="15">
+        <v>41</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="H15" s="15">
+        <v>261900</v>
+      </c>
+      <c r="I15" s="15">
+        <v>7.0087554701705255</v>
+      </c>
+      <c r="J15" s="15">
+        <v>68.02</v>
+      </c>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15">
+        <v>7.649</v>
+      </c>
+      <c r="N15" s="15">
+        <v>9.2416438149574509E-2</v>
+      </c>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15">
+        <v>0.33566000000000001</v>
+      </c>
+      <c r="Q15" s="15">
+        <v>1.4087571934942152E-4</v>
+      </c>
+      <c r="R15" s="15">
+        <v>2.5364843371633622E-3</v>
+      </c>
+      <c r="S15" s="15">
+        <v>5.5159451781937032E-3</v>
+      </c>
+      <c r="T15" s="15">
+        <v>1.9662301714565176E-3</v>
+      </c>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15">
+        <v>3.44696864137495E-3</v>
+      </c>
+      <c r="X15" s="15">
+        <v>2.2433994774168512E-4</v>
+      </c>
+      <c r="Y15" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z15" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="AA15" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="AB15" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15" t="s">
+        <v>433</v>
+      </c>
+      <c r="AF15" s="15" t="s">
+        <v>430</v>
+      </c>
+      <c r="AG15" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="AH15" s="15" t="s">
+        <v>433</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR115"/>
@@ -28954,11 +30149,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR283"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S37" sqref="S37"/>
+      <selection pane="bottomRight" sqref="A1:AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -29045,22 +30240,22 @@
       <c r="S1" s="40" t="s">
         <v>436</v>
       </c>
-      <c r="T1" s="46" t="s">
+      <c r="T1" s="42" t="s">
         <v>437</v>
       </c>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="42" t="s">
         <v>417</v>
       </c>
-      <c r="V1" s="46" t="s">
+      <c r="V1" s="42" t="s">
         <v>438</v>
       </c>
       <c r="W1" s="40" t="s">
         <v>439</v>
       </c>
-      <c r="X1" s="46" t="s">
+      <c r="X1" s="42" t="s">
         <v>440</v>
       </c>
-      <c r="Y1" s="46" t="s">
+      <c r="Y1" s="42" t="s">
         <v>162</v>
       </c>
       <c r="Z1" s="40" t="s">
@@ -50535,17 +51730,17 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="42" t="s">
+      <c r="A43" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="42"/>
+      <c r="B43" s="43"/>
     </row>
     <row r="44" spans="1:9" ht="15" thickBot="1"/>
     <row r="45" spans="1:9">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="43"/>
+      <c r="B45" s="44"/>
       <c r="C45" t="s">
         <v>238</v>
       </c>
@@ -58926,30 +60121,30 @@
       <c r="B2" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="44" t="s">
+      <c r="I2" s="46"/>
+      <c r="J2" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="44" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="M2" s="45"/>
-      <c r="N2" s="44" t="s">
+      <c r="M2" s="46"/>
+      <c r="N2" s="45" t="s">
         <v>491</v>
       </c>
-      <c r="O2" s="45"/>
-      <c r="P2" s="44" t="s">
+      <c r="O2" s="46"/>
+      <c r="P2" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="44" t="s">
+      <c r="Q2" s="46"/>
+      <c r="R2" s="45" t="s">
         <v>206</v>
       </c>
-      <c r="S2" s="45"/>
+      <c r="S2" s="46"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">

</xml_diff>